<commit_message>
New version of : README.MD
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TaiLieuHCMUS\BoschCodeRace\CodeRace_FinalRound\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bui nguyen hoang\Desktop\WorkSpace\Busitech\Bosch-CodeRace-Round4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26CA79B3-4CC8-473A-B303-EE93739920F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4EE3CF-DA4D-4ED8-9B1F-F2AD3596DB07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ArrayMapping" sheetId="5" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="92">
   <si>
     <t>Artifact Type</t>
   </si>
@@ -660,9 +660,6 @@
   </si>
   <si>
     <t>modified_on</t>
-  </si>
-  <si>
-    <t>title</t>
   </si>
   <si>
     <t>contributor</t>
@@ -1380,6 +1377,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1388,9 +1388,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2286,13 +2283,13 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
-    <col min="2" max="2" width="33.33203125" customWidth="1"/>
+    <col min="1" max="1" width="25.3046875" customWidth="1"/>
+    <col min="2" max="2" width="33.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -2300,7 +2297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -2326,18 +2323,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="50.33203125" customWidth="1"/>
-    <col min="3" max="3" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.84375" customWidth="1"/>
+    <col min="2" max="2" width="50.3046875" customWidth="1"/>
+    <col min="3" max="3" width="30.84375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -2348,7 +2345,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
@@ -2359,7 +2356,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -2370,7 +2367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -2381,7 +2378,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -2392,7 +2389,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -2403,7 +2400,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -2414,7 +2411,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -2425,7 +2422,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
@@ -2436,7 +2433,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
@@ -2447,7 +2444,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -2458,7 +2455,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" s="5" t="s">
         <v>9</v>
       </c>
@@ -2466,10 +2463,10 @@
         <v>9</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
@@ -2477,10 +2474,10 @@
         <v>11</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
@@ -2488,10 +2485,10 @@
         <v>12</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
         <v>13</v>
       </c>
@@ -2499,10 +2496,10 @@
         <v>13</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" s="7" t="s">
         <v>18</v>
       </c>
@@ -2510,7 +2507,7 @@
         <v>18</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2530,14 +2527,14 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="44.109375" customWidth="1"/>
-    <col min="3" max="3" width="65.5546875" customWidth="1"/>
+    <col min="1" max="1" width="15.69140625" customWidth="1"/>
+    <col min="2" max="2" width="44.07421875" customWidth="1"/>
+    <col min="3" max="3" width="65.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
@@ -2548,7 +2545,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -2559,7 +2556,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>20</v>
       </c>
@@ -2570,137 +2567,137 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -2734,17 +2731,17 @@
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="69.109375" customWidth="1"/>
+    <col min="1" max="1" width="69.07421875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>57</v>
       </c>
@@ -2767,13 +2764,13 @@
       <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="42.33203125" customWidth="1"/>
-    <col min="2" max="2" width="72.33203125" customWidth="1"/>
+    <col min="1" max="1" width="42.3046875" customWidth="1"/>
+    <col min="2" max="2" width="72.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2781,7 +2778,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="45.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="45.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
         <v>21</v>
       </c>
@@ -2789,7 +2786,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="41.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="41.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="9" t="s">
         <v>23</v>
       </c>
@@ -2797,7 +2794,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="50.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="50.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="9" t="s">
         <v>24</v>
       </c>
@@ -2805,7 +2802,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="50.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="9" t="s">
         <v>25</v>
       </c>
@@ -2834,13 +2831,13 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="45.6640625" customWidth="1"/>
-    <col min="2" max="2" width="49.21875" customWidth="1"/>
+    <col min="1" max="1" width="45.69140625" customWidth="1"/>
+    <col min="2" max="2" width="49.23046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -2848,7 +2845,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="str">
         <f>AttributeMapping!B2</f>
         <v>Attribute Type</v>
@@ -2857,7 +2854,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" s="9" t="str">
         <f>AttributeMapping!B3</f>
         <v>ReqIF.Text</v>
@@ -2866,7 +2863,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" s="9" t="str">
         <f>AttributeMapping!B4</f>
         <v>Status</v>
@@ -2875,7 +2872,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" s="9" t="str">
         <f>AttributeMapping!B5</f>
         <v>crq</v>
@@ -2884,7 +2881,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" s="9" t="str">
         <f>AttributeMapping!B6</f>
         <v>VAR_FUNC_SYS</v>
@@ -2893,7 +2890,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" s="9" t="str">
         <f>AttributeMapping!B7</f>
         <v>Allocation</v>
@@ -2902,7 +2899,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" s="9" t="str">
         <f>AttributeMapping!B8</f>
         <v>Safety Classification</v>
@@ -2911,7 +2908,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" s="9" t="str">
         <f>AttributeMapping!B9</f>
         <v>Verification Criteria</v>
@@ -2920,7 +2917,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A10" s="9" t="str">
         <f>AttributeMapping!B10</f>
         <v>Identifier</v>
@@ -2929,7 +2926,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A11" s="9" t="str">
         <f>AttributeMapping!B11</f>
         <v>Modified On</v>
@@ -2938,7 +2935,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A12" s="9" t="str">
         <f>AttributeMapping!B12</f>
         <v>Title</v>
@@ -2947,7 +2944,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A13" s="9" t="str">
         <f>AttributeMapping!B13</f>
         <v>Contributor</v>
@@ -2956,7 +2953,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A14" s="9" t="str">
         <f>AttributeMapping!B14</f>
         <v>Creator</v>
@@ -2965,7 +2962,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A15" s="9" t="str">
         <f>AttributeMapping!B15</f>
         <v>Description</v>
@@ -2974,7 +2971,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A16" s="9" t="str">
         <f>AttributeMapping!B16</f>
         <v>Created On</v>
@@ -3004,13 +3001,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="38.6640625" customWidth="1"/>
-    <col min="2" max="2" width="43.109375" customWidth="1"/>
+    <col min="1" max="1" width="38.69140625" customWidth="1"/>
+    <col min="2" max="2" width="43.07421875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>65</v>
       </c>
@@ -3018,7 +3015,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -3038,30 +3035,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7E12D30-BEF0-4150-8A7A-E27D1B2CE29F}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.21875" style="10"/>
-    <col min="2" max="2" width="21.5546875" style="10" customWidth="1"/>
-    <col min="3" max="3" width="52.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.23046875" style="10"/>
+    <col min="2" max="2" width="21.53515625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="52.07421875" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" style="10" customWidth="1"/>
-    <col min="5" max="5" width="76.6640625" style="10" customWidth="1"/>
-    <col min="6" max="16384" width="9.21875" style="10"/>
+    <col min="5" max="5" width="76.69140625" style="10" customWidth="1"/>
+    <col min="6" max="16384" width="9.23046875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A1" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="23"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="24"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" s="11" t="s">
         <v>41</v>
       </c>
@@ -3078,7 +3075,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="262.3" x14ac:dyDescent="0.4">
       <c r="A3" s="13">
         <v>1</v>
       </c>
@@ -3095,7 +3092,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A4" s="13">
         <v>2</v>
       </c>
@@ -3112,7 +3109,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A5" s="13">
         <v>3</v>
       </c>
@@ -3129,16 +3126,16 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="21" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A8" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="23"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="24"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" s="11" t="s">
         <v>41</v>
       </c>
@@ -3155,7 +3152,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A10" s="13">
         <v>1</v>
       </c>
@@ -3172,7 +3169,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A11" s="13">
         <v>2</v>
       </c>
@@ -3189,7 +3186,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A12" s="13">
         <v>3</v>
       </c>
@@ -3206,11 +3203,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A13" s="17">
         <v>4</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="21" t="s">
         <v>72</v>
       </c>
       <c r="C13" s="18" t="s">
@@ -3220,19 +3217,19 @@
         <v>38</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A16" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="23"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="24"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" s="11" t="s">
         <v>41</v>
       </c>
@@ -3249,7 +3246,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A18" s="13">
         <v>1</v>
       </c>

</xml_diff>